<commit_message>
Commit with bugs in the baseRunner and the score fixed
</commit_message>
<xml_diff>
--- a/Baseball/teams.xlsx
+++ b/Baseball/teams.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
   <si>
     <t>Black</t>
   </si>
@@ -178,40 +178,40 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M2" t="e">
-        <v>#NUM!</v>
+        <v>1.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="3">
@@ -261,13 +261,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" t="n">
         <v>0.0</v>
@@ -276,25 +276,29 @@
         <v>0.0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M4"/>
-      <c r="N4"/>
+        <v>5.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>3.6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -355,40 +359,40 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="E2" t="n">
         <v>0.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G2" t="n">
         <v>0.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M2" t="e">
-        <v>#NUM!</v>
+        <v>1.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="3">
@@ -438,40 +442,44 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D4" t="n">
         <v>0.0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" t="n">
         <v>0.0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M4"/>
-      <c r="N4"/>
+        <v>6.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>12.6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>